<commit_message>
Datos utilizados para la actualización 09/06/2021
</commit_message>
<xml_diff>
--- a/Datos_a_Junio/DESEMBARQUE.xlsx
+++ b/Datos_a_Junio/DESEMBARQUE.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariajosezunigabasualto/MJZ/CTP2021/SARDINA_AUSTRAL LOS LAGOS/INFORME_FINAL/Datos_a_Junio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E1B83A-4F81-0440-A8DD-CDF1B1DBBBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DE175C-873B-934C-9E51-170536A2C33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="500" windowWidth="21860" windowHeight="26820" activeTab="2" xr2:uid="{D73FE552-5237-42B3-AA1B-489DDDA3A168}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="25340" windowHeight="26820" activeTab="2" xr2:uid="{D73FE552-5237-42B3-AA1B-489DDDA3A168}"/>
   </bookViews>
   <sheets>
     <sheet name="XI Region " sheetId="2" r:id="rId1"/>
     <sheet name="X Region" sheetId="1" r:id="rId2"/>
-    <sheet name="MES" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId3"/>
+    <sheet name="MES" sheetId="3" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'X Region'!$B$2:$G$62</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="35">
   <si>
     <t>Evolución de las capturas de las principales especies,</t>
   </si>
@@ -137,6 +138,18 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>desemb + descarte</t>
+  </si>
+  <si>
+    <t>%descarte</t>
+  </si>
+  <si>
+    <t>Corregir esta serie en PRIMER INFORME SEPTIEMBRE 2021</t>
+  </si>
+  <si>
+    <t># Frecuencia_cruceros</t>
+  </si>
 </sst>
 </file>
 
@@ -191,7 +204,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,6 +232,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -391,7 +410,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -504,6 +523,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -519,9 +541,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4717,24 +4761,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
+      <c r="B2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="5" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="6" t="s">
@@ -5092,14 +5136,14 @@
       </c>
     </row>
     <row r="65" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B65" s="40" t="s">
+      <c r="B65" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C65" s="40"/>
-      <c r="D65" s="40"/>
-      <c r="E65" s="40"/>
-      <c r="F65" s="40"/>
-      <c r="G65" s="40"/>
+      <c r="C65" s="41"/>
+      <c r="D65" s="41"/>
+      <c r="E65" s="41"/>
+      <c r="F65" s="41"/>
+      <c r="G65" s="41"/>
     </row>
     <row r="66" spans="2:7" s="2" customFormat="1" ht="8.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B66" s="25"/>
@@ -5128,10 +5172,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:Q64"/>
+  <dimension ref="B2:AD64"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L49" sqref="L49"/>
+    <sheetView showGridLines="0" topLeftCell="O8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5151,14 +5195,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
+      <c r="B2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
       <c r="H2" s="1"/>
       <c r="J2" s="3" t="s">
         <v>1</v>
@@ -5169,14 +5213,14 @@
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
       <c r="H3" s="1"/>
     </row>
     <row r="5" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -5442,7 +5486,7 @@
       </c>
       <c r="H16" s="17"/>
     </row>
-    <row r="17" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="14">
         <v>2016</v>
       </c>
@@ -5464,7 +5508,7 @@
       </c>
       <c r="H17" s="17"/>
     </row>
-    <row r="18" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="14">
         <v>2017</v>
       </c>
@@ -5486,7 +5530,7 @@
       </c>
       <c r="H18" s="17"/>
     </row>
-    <row r="19" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="14">
         <v>2018</v>
       </c>
@@ -5508,7 +5552,7 @@
       </c>
       <c r="H19" s="17"/>
     </row>
-    <row r="20" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="14">
         <v>2019</v>
       </c>
@@ -5528,8 +5572,15 @@
         <v>13218.897000000001</v>
       </c>
       <c r="H20" s="17"/>
-    </row>
-    <row r="21" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R20" s="46"/>
+      <c r="S20" s="46"/>
+      <c r="T20" s="46"/>
+      <c r="U20" s="46"/>
+      <c r="V20" s="46"/>
+      <c r="W20" s="46"/>
+      <c r="X20" s="46"/>
+    </row>
+    <row r="21" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="26">
         <v>2020</v>
       </c>
@@ -5566,8 +5617,12 @@
       <c r="O21" s="20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="2:15" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S21" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="X21" s="5"/>
+    </row>
+    <row r="22" spans="2:25" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="21"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
@@ -5575,333 +5630,899 @@
       <c r="F22" s="22"/>
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
-    </row>
-    <row r="23" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R22" s="47"/>
+      <c r="S22" s="47"/>
+      <c r="T22" s="48"/>
+      <c r="U22" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="V22" s="48"/>
+      <c r="W22" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="X22" s="5"/>
+    </row>
+    <row r="23" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K23" s="4">
         <v>2001</v>
       </c>
-      <c r="M23" s="4">
+      <c r="L23" s="44"/>
+      <c r="M23" s="44">
         <v>5921.0780000000004</v>
       </c>
-      <c r="N23" s="4">
+      <c r="N23" s="44">
         <v>361.048</v>
       </c>
-      <c r="O23" s="4">
+      <c r="O23" s="44">
         <v>6018.9989999999998</v>
       </c>
-    </row>
-    <row r="24" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P23" s="44">
+        <f>+L23+M23+N23</f>
+        <v>6282.1260000000002</v>
+      </c>
+      <c r="R23" s="49">
+        <v>2002</v>
+      </c>
+      <c r="S23" s="49">
+        <v>38974</v>
+      </c>
+      <c r="T23" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U23" s="50">
+        <f>+T23/100</f>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V23" s="50">
+        <f>1+U23</f>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W23" s="51">
+        <f>+S23*V23</f>
+        <v>39878.196800000005</v>
+      </c>
+      <c r="X23" s="50"/>
+      <c r="Y23" s="49"/>
+    </row>
+    <row r="24" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K24" s="4">
         <v>2002</v>
       </c>
-      <c r="M24" s="4">
+      <c r="L24" s="44"/>
+      <c r="M24" s="44">
         <v>6396.3639999999996</v>
       </c>
-      <c r="N24" s="4">
+      <c r="N24" s="44">
         <v>3026.1770000000001</v>
       </c>
-      <c r="O24" s="4">
+      <c r="O24" s="44">
         <v>5276.5309999999999</v>
       </c>
-    </row>
-    <row r="25" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P24" s="44">
+        <f t="shared" ref="P24:P42" si="1">+L24+M24+N24</f>
+        <v>9422.5409999999993</v>
+      </c>
+      <c r="R24" s="49">
+        <v>2003</v>
+      </c>
+      <c r="S24" s="49">
+        <v>32843</v>
+      </c>
+      <c r="T24" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U24" s="50">
+        <f t="shared" ref="U24:U42" si="2">+T24/100</f>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V24" s="50">
+        <f t="shared" ref="V24:V42" si="3">1+U24</f>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W24" s="51">
+        <f t="shared" ref="W24:W42" si="4">+S24*V24</f>
+        <v>33604.957600000002</v>
+      </c>
+      <c r="X24" s="50"/>
+      <c r="Y24" s="49"/>
+    </row>
+    <row r="25" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K25" s="4">
         <v>2003</v>
       </c>
-      <c r="M25" s="4">
+      <c r="L25" s="44"/>
+      <c r="M25" s="44">
         <v>19703.317999999999</v>
       </c>
-      <c r="N25" s="4">
+      <c r="N25" s="44">
         <v>5382.94</v>
       </c>
-      <c r="O25" s="4">
+      <c r="O25" s="44">
         <v>4521.817</v>
       </c>
-    </row>
-    <row r="26" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P25" s="44">
+        <f t="shared" si="1"/>
+        <v>25086.257999999998</v>
+      </c>
+      <c r="R25" s="49">
+        <v>2004</v>
+      </c>
+      <c r="S25" s="49">
+        <v>36545</v>
+      </c>
+      <c r="T25" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U25" s="50">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V25" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W25" s="51">
+        <f t="shared" si="4"/>
+        <v>37392.844000000005</v>
+      </c>
+      <c r="X25" s="50"/>
+      <c r="Y25" s="49"/>
+    </row>
+    <row r="26" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K26" s="4">
         <v>2004</v>
       </c>
-      <c r="M26" s="4">
+      <c r="L26" s="44"/>
+      <c r="M26" s="44">
         <v>19234.650000000001</v>
       </c>
-      <c r="N26" s="4">
+      <c r="N26" s="44">
         <v>8590.5159999999996</v>
       </c>
-      <c r="O26" s="4">
+      <c r="O26" s="44">
         <v>4289.7179999999998</v>
       </c>
-    </row>
-    <row r="27" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P26" s="44">
+        <f t="shared" si="1"/>
+        <v>27825.166000000001</v>
+      </c>
+      <c r="R26" s="49">
+        <v>2005</v>
+      </c>
+      <c r="S26" s="49">
+        <v>52569</v>
+      </c>
+      <c r="T26" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U26" s="50">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V26" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W26" s="51">
+        <f t="shared" si="4"/>
+        <v>53788.600800000007</v>
+      </c>
+      <c r="X26" s="50"/>
+      <c r="Y26" s="49"/>
+    </row>
+    <row r="27" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K27" s="4">
         <v>2005</v>
       </c>
-      <c r="M27" s="4">
+      <c r="L27" s="44"/>
+      <c r="M27" s="44">
         <v>18049.284</v>
       </c>
-      <c r="N27" s="4">
+      <c r="N27" s="44">
         <v>5127.1589999999997</v>
       </c>
-      <c r="O27" s="4">
+      <c r="O27" s="44">
         <v>1841.71</v>
       </c>
-    </row>
-    <row r="28" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P27" s="44">
+        <f t="shared" si="1"/>
+        <v>23176.442999999999</v>
+      </c>
+      <c r="R27" s="49">
+        <v>2006</v>
+      </c>
+      <c r="S27" s="49">
+        <v>39146</v>
+      </c>
+      <c r="T27" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U27" s="50">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V27" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W27" s="51">
+        <f t="shared" si="4"/>
+        <v>40054.187200000008</v>
+      </c>
+      <c r="X27" s="50"/>
+      <c r="Y27" s="49"/>
+    </row>
+    <row r="28" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K28" s="4">
         <v>2006</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28" s="44">
         <v>35959.404000000002</v>
       </c>
-      <c r="M28" s="4">
+      <c r="M28" s="44">
         <v>1417.2090000000001</v>
       </c>
-      <c r="N28" s="4">
+      <c r="N28" s="44">
         <v>4468.2460000000001</v>
       </c>
-      <c r="O28" s="4">
+      <c r="O28" s="44">
         <v>327.48</v>
       </c>
-    </row>
-    <row r="29" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P28" s="44">
+        <f t="shared" si="1"/>
+        <v>41844.859000000004</v>
+      </c>
+      <c r="R28" s="49">
+        <v>2007</v>
+      </c>
+      <c r="S28" s="49">
+        <v>50506</v>
+      </c>
+      <c r="T28" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U28" s="50">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V28" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W28" s="51">
+        <f t="shared" si="4"/>
+        <v>51677.739200000004</v>
+      </c>
+      <c r="X28" s="50"/>
+      <c r="Y28" s="49"/>
+    </row>
+    <row r="29" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K29" s="4">
         <v>2007</v>
       </c>
-      <c r="L29" s="4">
+      <c r="L29" s="44">
         <v>44473.264999999999</v>
       </c>
-      <c r="M29" s="4">
+      <c r="M29" s="44">
         <v>4215.8500000000004</v>
       </c>
-      <c r="N29" s="4">
+      <c r="N29" s="44">
         <v>8161.2539999999999</v>
       </c>
-      <c r="O29" s="4">
+      <c r="O29" s="44">
         <v>45.496000000000002</v>
       </c>
-    </row>
-    <row r="30" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P29" s="44">
+        <f t="shared" si="1"/>
+        <v>56850.368999999999</v>
+      </c>
+      <c r="R29" s="49">
+        <v>2008</v>
+      </c>
+      <c r="S29" s="49">
+        <v>45078</v>
+      </c>
+      <c r="T29" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U29" s="50">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V29" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W29" s="51">
+        <f t="shared" si="4"/>
+        <v>46123.809600000008</v>
+      </c>
+      <c r="X29" s="50"/>
+      <c r="Y29" s="49"/>
+    </row>
+    <row r="30" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K30" s="4">
         <v>2008</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30" s="44">
         <v>45079.665000000001</v>
       </c>
-      <c r="M30" s="4">
+      <c r="M30" s="44">
         <v>14420.11</v>
       </c>
-      <c r="N30" s="4">
+      <c r="N30" s="44">
         <v>10440.206</v>
       </c>
-      <c r="O30" s="4">
+      <c r="O30" s="44">
         <v>1146.76</v>
       </c>
-    </row>
-    <row r="31" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P30" s="44">
+        <f t="shared" si="1"/>
+        <v>69939.981</v>
+      </c>
+      <c r="R30" s="49">
+        <v>2009</v>
+      </c>
+      <c r="S30" s="49">
+        <v>49225</v>
+      </c>
+      <c r="T30" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U30" s="50">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V30" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W30" s="51">
+        <f t="shared" si="4"/>
+        <v>50367.020000000004</v>
+      </c>
+      <c r="X30" s="50"/>
+      <c r="Y30" s="49"/>
+    </row>
+    <row r="31" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K31" s="4">
         <v>2009</v>
       </c>
-      <c r="L31" s="4">
+      <c r="L31" s="44">
         <v>49222.15</v>
       </c>
-      <c r="M31" s="4">
+      <c r="M31" s="44">
         <v>18551.712</v>
       </c>
-      <c r="N31" s="4">
+      <c r="N31" s="44">
         <v>9688.0450000000001</v>
       </c>
-      <c r="O31" s="4">
+      <c r="O31" s="44">
         <v>295.654</v>
       </c>
-    </row>
-    <row r="32" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P31" s="44">
+        <f t="shared" si="1"/>
+        <v>77461.906999999992</v>
+      </c>
+      <c r="R31" s="49">
+        <v>2010</v>
+      </c>
+      <c r="S31" s="49">
+        <v>20123</v>
+      </c>
+      <c r="T31" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U31" s="50">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V31" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W31" s="51">
+        <f t="shared" si="4"/>
+        <v>20589.853600000002</v>
+      </c>
+      <c r="X31" s="50"/>
+      <c r="Y31" s="49"/>
+    </row>
+    <row r="32" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K32" s="4">
         <v>2010</v>
       </c>
-      <c r="L32" s="4">
+      <c r="L32" s="44">
         <v>20224.114000000001</v>
       </c>
-      <c r="M32" s="4">
+      <c r="M32" s="44">
         <v>11233.092000000001</v>
       </c>
-      <c r="N32" s="4">
+      <c r="N32" s="44">
         <v>2804.5709999999999</v>
       </c>
-      <c r="O32" s="4">
+      <c r="O32" s="44">
         <v>686.46699999999998</v>
       </c>
-    </row>
-    <row r="33" spans="11:17" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P32" s="44">
+        <f t="shared" si="1"/>
+        <v>34261.777000000002</v>
+      </c>
+      <c r="R32" s="49">
+        <v>2011</v>
+      </c>
+      <c r="S32" s="49">
+        <v>16429</v>
+      </c>
+      <c r="T32" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U32" s="50">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V32" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W32" s="51">
+        <f t="shared" si="4"/>
+        <v>16810.152800000003</v>
+      </c>
+      <c r="X32" s="50"/>
+      <c r="Y32" s="49"/>
+    </row>
+    <row r="33" spans="11:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K33" s="4">
         <v>2011</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L33" s="44">
         <v>16793.392</v>
       </c>
-      <c r="M33" s="4">
+      <c r="M33" s="44">
         <v>7213.6980000000003</v>
       </c>
-      <c r="N33" s="4">
+      <c r="N33" s="44">
         <v>1766.722</v>
       </c>
-      <c r="O33" s="4">
+      <c r="O33" s="44">
         <v>695.03</v>
       </c>
-    </row>
-    <row r="34" spans="11:17" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P33" s="44">
+        <f t="shared" si="1"/>
+        <v>25773.812000000002</v>
+      </c>
+      <c r="R33" s="49">
+        <v>2012</v>
+      </c>
+      <c r="S33" s="49">
+        <v>19763</v>
+      </c>
+      <c r="T33" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U33" s="50">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V33" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W33" s="51">
+        <f t="shared" si="4"/>
+        <v>20221.501600000003</v>
+      </c>
+      <c r="X33" s="50"/>
+      <c r="Y33" s="49"/>
+    </row>
+    <row r="34" spans="11:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K34" s="4">
         <v>2012</v>
       </c>
-      <c r="L34" s="4">
+      <c r="L34" s="44">
         <v>19719.138999999999</v>
       </c>
-      <c r="M34" s="4">
+      <c r="M34" s="44">
         <v>19181.367999999999</v>
       </c>
-      <c r="N34" s="4">
+      <c r="N34" s="44">
         <v>962.83399999999995</v>
       </c>
-      <c r="O34" s="4">
+      <c r="O34" s="44">
         <v>544.351</v>
       </c>
-    </row>
-    <row r="35" spans="11:17" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P34" s="44">
+        <f t="shared" si="1"/>
+        <v>39863.341</v>
+      </c>
+      <c r="R34" s="49">
+        <v>2013</v>
+      </c>
+      <c r="S34" s="49">
+        <v>21888</v>
+      </c>
+      <c r="T34" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U34" s="50">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V34" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W34" s="51">
+        <f t="shared" si="4"/>
+        <v>22395.801600000003</v>
+      </c>
+      <c r="X34" s="50"/>
+      <c r="Y34" s="49"/>
+    </row>
+    <row r="35" spans="11:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K35" s="4">
         <v>2013</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L35" s="44">
         <v>21751.952000000001</v>
       </c>
-      <c r="M35" s="4">
+      <c r="M35" s="44">
         <v>4295.9210000000003</v>
       </c>
-      <c r="N35" s="4">
+      <c r="N35" s="44">
         <v>618.69799999999998</v>
       </c>
-      <c r="O35" s="4">
+      <c r="O35" s="44">
         <v>349.02499999999998</v>
       </c>
-    </row>
-    <row r="36" spans="11:17" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P35" s="44">
+        <f t="shared" si="1"/>
+        <v>26666.571</v>
+      </c>
+      <c r="R35" s="49">
+        <v>2014</v>
+      </c>
+      <c r="S35" s="49">
+        <v>22951</v>
+      </c>
+      <c r="T35" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U35" s="50">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V35" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W35" s="51">
+        <f t="shared" si="4"/>
+        <v>23483.463200000002</v>
+      </c>
+      <c r="X35" s="50"/>
+      <c r="Y35" s="49"/>
+    </row>
+    <row r="36" spans="11:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K36" s="4">
         <v>2014</v>
       </c>
-      <c r="L36" s="4">
+      <c r="L36" s="44">
         <v>22778.775000000001</v>
       </c>
-      <c r="M36" s="4">
+      <c r="M36" s="44">
         <v>1283.7760000000001</v>
       </c>
-      <c r="N36" s="4">
+      <c r="N36" s="44">
         <v>292.34699999999998</v>
       </c>
-      <c r="O36" s="4">
+      <c r="O36" s="44">
         <v>43.912999999999997</v>
       </c>
-    </row>
-    <row r="37" spans="11:17" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P36" s="44">
+        <f t="shared" si="1"/>
+        <v>24354.898000000005</v>
+      </c>
+      <c r="R36" s="49">
+        <v>2015</v>
+      </c>
+      <c r="S36" s="49">
+        <v>23643</v>
+      </c>
+      <c r="T36" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U36" s="50">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V36" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W36" s="51">
+        <f t="shared" si="4"/>
+        <v>24191.517600000003</v>
+      </c>
+      <c r="X36" s="50"/>
+      <c r="Y36" s="49"/>
+    </row>
+    <row r="37" spans="11:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K37" s="4">
         <v>2015</v>
       </c>
-      <c r="L37" s="4">
+      <c r="L37" s="44">
         <v>23710.723000000002</v>
       </c>
-      <c r="M37" s="4">
+      <c r="M37" s="44">
         <v>1026.7139999999999</v>
       </c>
-      <c r="N37" s="4">
+      <c r="N37" s="44">
         <v>642.73400000000004</v>
       </c>
-      <c r="O37" s="4">
+      <c r="O37" s="44">
         <v>27.45</v>
       </c>
-    </row>
-    <row r="38" spans="11:17" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P37" s="44">
+        <f t="shared" si="1"/>
+        <v>25380.171000000002</v>
+      </c>
+      <c r="R37" s="49">
+        <v>2016</v>
+      </c>
+      <c r="S37" s="49">
+        <v>18495</v>
+      </c>
+      <c r="T37" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U37" s="50">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V37" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W37" s="51">
+        <f t="shared" si="4"/>
+        <v>18924.084000000003</v>
+      </c>
+      <c r="X37" s="50"/>
+      <c r="Y37" s="49"/>
+    </row>
+    <row r="38" spans="11:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K38" s="4">
         <v>2016</v>
       </c>
-      <c r="L38" s="4">
+      <c r="L38" s="44">
         <v>18473.806</v>
       </c>
-      <c r="M38" s="4">
+      <c r="M38" s="44">
         <v>2832.0250000000001</v>
       </c>
-      <c r="N38" s="4">
+      <c r="N38" s="44">
         <v>1658.192</v>
       </c>
-      <c r="O38" s="4">
+      <c r="O38" s="44">
         <v>243.53200000000001</v>
       </c>
-    </row>
-    <row r="39" spans="11:17" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P38" s="44">
+        <f t="shared" si="1"/>
+        <v>22964.023000000001</v>
+      </c>
+      <c r="R38" s="49">
+        <v>2017</v>
+      </c>
+      <c r="S38" s="49">
+        <v>14134</v>
+      </c>
+      <c r="T38" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U38" s="50">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V38" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W38" s="51">
+        <f t="shared" si="4"/>
+        <v>14461.908800000001</v>
+      </c>
+      <c r="X38" s="50"/>
+      <c r="Y38" s="49"/>
+    </row>
+    <row r="39" spans="11:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K39" s="4">
         <v>2017</v>
       </c>
-      <c r="L39" s="4">
+      <c r="L39" s="44">
         <v>14133.52</v>
       </c>
-      <c r="M39" s="4">
+      <c r="M39" s="44">
         <v>6012.82</v>
       </c>
-      <c r="N39" s="4">
+      <c r="N39" s="44">
         <v>1474.9010000000001</v>
       </c>
-      <c r="O39" s="4">
+      <c r="O39" s="44">
         <v>16.792999999999999</v>
       </c>
-    </row>
-    <row r="40" spans="11:17" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P39" s="44">
+        <f t="shared" si="1"/>
+        <v>21621.241000000002</v>
+      </c>
+      <c r="R39" s="49">
+        <v>2018</v>
+      </c>
+      <c r="S39" s="49">
+        <v>8355</v>
+      </c>
+      <c r="T39" s="50">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="U39" s="50">
+        <f t="shared" si="2"/>
+        <v>4.8600000000000004E-2</v>
+      </c>
+      <c r="V39" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0486</v>
+      </c>
+      <c r="W39" s="51">
+        <f t="shared" si="4"/>
+        <v>8761.0529999999999</v>
+      </c>
+      <c r="X39" s="50"/>
+      <c r="Y39" s="49"/>
+    </row>
+    <row r="40" spans="11:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K40" s="4">
         <v>2018</v>
       </c>
-      <c r="L40" s="4">
+      <c r="L40" s="44">
         <v>8355.3649999999998</v>
       </c>
-      <c r="M40" s="4">
+      <c r="M40" s="44">
         <v>669.31799999999998</v>
       </c>
-      <c r="N40" s="4">
+      <c r="N40" s="44">
         <v>395.56099999999998</v>
       </c>
-      <c r="O40" s="4">
+      <c r="O40" s="44">
         <v>82.227000000000004</v>
       </c>
-    </row>
-    <row r="41" spans="11:17" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P40" s="44">
+        <f t="shared" si="1"/>
+        <v>9420.2439999999988</v>
+      </c>
+      <c r="R40" s="49">
+        <v>2019</v>
+      </c>
+      <c r="S40" s="49">
+        <v>11278</v>
+      </c>
+      <c r="T40" s="50">
+        <v>0.93</v>
+      </c>
+      <c r="U40" s="50">
+        <f t="shared" si="2"/>
+        <v>9.300000000000001E-3</v>
+      </c>
+      <c r="V40" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0093000000000001</v>
+      </c>
+      <c r="W40" s="51">
+        <f t="shared" si="4"/>
+        <v>11382.885400000001</v>
+      </c>
+      <c r="X40" s="50"/>
+      <c r="Y40" s="49"/>
+    </row>
+    <row r="41" spans="11:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K41" s="4">
         <v>2019</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L41" s="44">
         <v>8017.7120000000004</v>
       </c>
-      <c r="M41" s="4">
+      <c r="M41" s="44">
         <v>530.82399999999996</v>
       </c>
-      <c r="N41" s="4">
+      <c r="N41" s="44">
         <v>1061.5229999999999</v>
       </c>
-      <c r="O41" s="4">
+      <c r="O41" s="44">
         <v>121.89700000000001</v>
       </c>
-    </row>
-    <row r="42" spans="11:17" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P41" s="44">
+        <f t="shared" si="1"/>
+        <v>9610.0589999999993</v>
+      </c>
+      <c r="R41" s="49">
+        <v>2020</v>
+      </c>
+      <c r="S41" s="49">
+        <v>14194</v>
+      </c>
+      <c r="T41" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U41" s="50">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V41" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W41" s="51">
+        <f t="shared" si="4"/>
+        <v>14523.300800000001</v>
+      </c>
+      <c r="X41" s="49"/>
+      <c r="Y41" s="49"/>
+    </row>
+    <row r="42" spans="11:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K42" s="4">
         <v>2020</v>
       </c>
-      <c r="L42" s="4">
+      <c r="L42" s="44">
         <v>14193.737999999999</v>
       </c>
-      <c r="M42" s="4">
+      <c r="M42" s="44">
         <v>1731.075</v>
       </c>
-      <c r="N42" s="4">
+      <c r="N42" s="44">
         <v>2615.7930000000001</v>
       </c>
-      <c r="O42" s="4">
+      <c r="O42" s="44">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="44" spans="11:17" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P42" s="44">
+        <f t="shared" si="1"/>
+        <v>18540.606</v>
+      </c>
+      <c r="R42" s="49">
+        <v>2021</v>
+      </c>
+      <c r="S42" s="49">
+        <v>12347</v>
+      </c>
+      <c r="T42" s="50">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="U42" s="50">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="V42" s="50">
+        <f t="shared" si="3"/>
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="W42" s="51">
+        <f t="shared" si="4"/>
+        <v>12633.450400000002</v>
+      </c>
+      <c r="X42" s="49"/>
+      <c r="Y42" s="49"/>
+    </row>
+    <row r="43" spans="11:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R43" s="49"/>
+      <c r="S43" s="49"/>
+      <c r="T43" s="49"/>
+      <c r="U43" s="49"/>
+      <c r="V43" s="49"/>
+      <c r="W43" s="49"/>
+      <c r="X43" s="49"/>
+      <c r="Y43" s="49"/>
+    </row>
+    <row r="44" spans="11:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K44" s="29"/>
       <c r="L44" s="29"/>
       <c r="M44" s="29"/>
@@ -5910,7 +6531,7 @@
       <c r="P44" s="29"/>
       <c r="Q44" s="29"/>
     </row>
-    <row r="45" spans="11:17" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="11:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K45" s="30"/>
       <c r="L45" s="30"/>
       <c r="M45" s="30"/>
@@ -5918,8 +6539,20 @@
       <c r="O45" s="31"/>
       <c r="P45" s="31"/>
       <c r="Q45" s="31"/>
-    </row>
-    <row r="46" spans="11:17" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AA45" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD45" s="4">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="46" spans="11:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K46" s="31"/>
       <c r="L46" s="31"/>
       <c r="M46" s="31"/>
@@ -5928,18 +6561,184 @@
       <c r="P46" s="31"/>
       <c r="Q46" s="31"/>
     </row>
-    <row r="62" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B62" s="41" t="s">
+    <row r="50" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AA50" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB50" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC50" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="AD50" s="4">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="52" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AA52" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB52" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC52" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="AD52" s="4">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="53" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AA53" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB53" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC53" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="AD53" s="4">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="54" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AA54" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB54" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC54" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="AD54" s="4">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="55" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AA55" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB55" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC55" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="AD55" s="4">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="56" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AA56" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB56" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC56" s="4">
+        <v>0.42</v>
+      </c>
+      <c r="AD56" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="57" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AA57" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB57" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC57" s="4">
+        <v>0.42</v>
+      </c>
+      <c r="AD57" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="58" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AA58" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB58" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC58" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="AD58" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="59" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AA59" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB59" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC59" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="AD59" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="60" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AA60" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB60" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC60" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="AD60" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="61" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AA61" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB61" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC61" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="AD61" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="62" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B62" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C62" s="42"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="42"/>
-      <c r="F62" s="42"/>
-      <c r="G62" s="42"/>
+      <c r="C62" s="43"/>
+      <c r="D62" s="43"/>
+      <c r="E62" s="43"/>
+      <c r="F62" s="43"/>
+      <c r="G62" s="43"/>
       <c r="H62" s="24"/>
-    </row>
-    <row r="63" spans="2:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AA62" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB62" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC62" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="AD62" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="63" spans="2:30" ht="6.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B63" s="24"/>
       <c r="C63" s="24"/>
       <c r="D63" s="24"/>
@@ -5947,9 +6746,33 @@
       <c r="F63" s="24"/>
       <c r="G63" s="24"/>
       <c r="H63" s="24"/>
-    </row>
-    <row r="64" spans="2:8" s="2" customFormat="1" ht="8.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AA63" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB63" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC63" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="AD63" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="64" spans="2:30" s="2" customFormat="1" ht="8.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B64" s="25"/>
+      <c r="AA64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC64" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="AD64" s="2">
+        <v>0.31</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5974,10 +6797,1870 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3B7E15-FD3C-DE4F-B81D-0C82D136DD2E}">
+  <dimension ref="A1:AD21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:AD22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0.01</v>
+      </c>
+      <c r="K6">
+        <v>0.08</v>
+      </c>
+      <c r="L6">
+        <v>0.08</v>
+      </c>
+      <c r="M6">
+        <v>0.12</v>
+      </c>
+      <c r="N6">
+        <v>0.13</v>
+      </c>
+      <c r="O6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="P6">
+        <v>0.04</v>
+      </c>
+      <c r="Q6">
+        <v>0.03</v>
+      </c>
+      <c r="R6">
+        <v>0.04</v>
+      </c>
+      <c r="S6">
+        <v>0.08</v>
+      </c>
+      <c r="T6">
+        <v>0.1</v>
+      </c>
+      <c r="U6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V6">
+        <v>0.05</v>
+      </c>
+      <c r="W6">
+        <v>0.02</v>
+      </c>
+      <c r="X6">
+        <v>0.01</v>
+      </c>
+      <c r="Y6">
+        <v>0.01</v>
+      </c>
+      <c r="Z6">
+        <v>0.01</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0.01</v>
+      </c>
+      <c r="E8">
+        <v>0.02</v>
+      </c>
+      <c r="F8">
+        <v>0.03</v>
+      </c>
+      <c r="G8">
+        <v>0.04</v>
+      </c>
+      <c r="H8">
+        <v>0.05</v>
+      </c>
+      <c r="I8">
+        <v>0.06</v>
+      </c>
+      <c r="J8">
+        <v>0.06</v>
+      </c>
+      <c r="K8">
+        <v>0.05</v>
+      </c>
+      <c r="L8">
+        <v>0.04</v>
+      </c>
+      <c r="M8">
+        <v>0.03</v>
+      </c>
+      <c r="N8">
+        <v>0.02</v>
+      </c>
+      <c r="O8">
+        <v>0.01</v>
+      </c>
+      <c r="P8">
+        <v>0.01</v>
+      </c>
+      <c r="Q8">
+        <v>0.01</v>
+      </c>
+      <c r="R8">
+        <v>0.02</v>
+      </c>
+      <c r="S8">
+        <v>0.03</v>
+      </c>
+      <c r="T8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U8">
+        <v>0.1</v>
+      </c>
+      <c r="V8">
+        <v>0.1</v>
+      </c>
+      <c r="W8">
+        <v>0.1</v>
+      </c>
+      <c r="X8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y8">
+        <v>0.03</v>
+      </c>
+      <c r="Z8">
+        <v>0.02</v>
+      </c>
+      <c r="AA8">
+        <v>0.01</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>0.01</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0.02</v>
+      </c>
+      <c r="H11">
+        <v>0.03</v>
+      </c>
+      <c r="I11">
+        <v>0.04</v>
+      </c>
+      <c r="J11">
+        <v>0.11</v>
+      </c>
+      <c r="K11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L11">
+        <v>0.11</v>
+      </c>
+      <c r="M11">
+        <v>0.06</v>
+      </c>
+      <c r="N11">
+        <v>0.06</v>
+      </c>
+      <c r="O11">
+        <v>0.08</v>
+      </c>
+      <c r="P11">
+        <v>0.08</v>
+      </c>
+      <c r="Q11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S11">
+        <v>0.06</v>
+      </c>
+      <c r="T11">
+        <v>0.03</v>
+      </c>
+      <c r="U11">
+        <v>0.01</v>
+      </c>
+      <c r="V11">
+        <v>0.01</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0.01</v>
+      </c>
+      <c r="I13">
+        <v>0.02</v>
+      </c>
+      <c r="J13">
+        <v>0.02</v>
+      </c>
+      <c r="K13">
+        <v>0.02</v>
+      </c>
+      <c r="L13">
+        <v>0.02</v>
+      </c>
+      <c r="M13">
+        <v>0.04</v>
+      </c>
+      <c r="N13">
+        <v>0.06</v>
+      </c>
+      <c r="O13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P13">
+        <v>0.12</v>
+      </c>
+      <c r="Q13">
+        <v>0.1</v>
+      </c>
+      <c r="R13">
+        <v>0.17</v>
+      </c>
+      <c r="S13">
+        <v>0.11</v>
+      </c>
+      <c r="T13">
+        <v>0.1</v>
+      </c>
+      <c r="U13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V13">
+        <v>0.05</v>
+      </c>
+      <c r="W13">
+        <v>0.02</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>0.02</v>
+      </c>
+      <c r="B14">
+        <v>0.05</v>
+      </c>
+      <c r="C14">
+        <v>0.06</v>
+      </c>
+      <c r="D14">
+        <v>0.08</v>
+      </c>
+      <c r="E14">
+        <v>0.13</v>
+      </c>
+      <c r="F14">
+        <v>0.11</v>
+      </c>
+      <c r="G14">
+        <v>0.1</v>
+      </c>
+      <c r="H14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I14">
+        <v>0.06</v>
+      </c>
+      <c r="J14">
+        <v>0.04</v>
+      </c>
+      <c r="K14">
+        <v>0.01</v>
+      </c>
+      <c r="L14">
+        <v>0.01</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0.01</v>
+      </c>
+      <c r="R14">
+        <v>0.01</v>
+      </c>
+      <c r="S14">
+        <v>0.02</v>
+      </c>
+      <c r="T14">
+        <v>0.04</v>
+      </c>
+      <c r="U14">
+        <v>0.05</v>
+      </c>
+      <c r="V14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W14">
+        <v>0.04</v>
+      </c>
+      <c r="X14">
+        <v>0.02</v>
+      </c>
+      <c r="Y14">
+        <v>0.01</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>0.01</v>
+      </c>
+      <c r="B15">
+        <v>0.02</v>
+      </c>
+      <c r="C15">
+        <v>0.04</v>
+      </c>
+      <c r="D15">
+        <v>0.03</v>
+      </c>
+      <c r="E15">
+        <v>0.04</v>
+      </c>
+      <c r="F15">
+        <v>0.03</v>
+      </c>
+      <c r="G15">
+        <v>0.03</v>
+      </c>
+      <c r="H15">
+        <v>0.04</v>
+      </c>
+      <c r="I15">
+        <v>0.05</v>
+      </c>
+      <c r="J15">
+        <v>0.06</v>
+      </c>
+      <c r="K15">
+        <v>0.04</v>
+      </c>
+      <c r="L15">
+        <v>0.02</v>
+      </c>
+      <c r="M15">
+        <v>0.04</v>
+      </c>
+      <c r="N15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O15">
+        <v>0.08</v>
+      </c>
+      <c r="P15">
+        <v>0.08</v>
+      </c>
+      <c r="Q15">
+        <v>0.06</v>
+      </c>
+      <c r="R15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T15">
+        <v>0.05</v>
+      </c>
+      <c r="U15">
+        <v>0.04</v>
+      </c>
+      <c r="V15">
+        <v>0.01</v>
+      </c>
+      <c r="W15">
+        <v>0.01</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0.1</v>
+      </c>
+      <c r="E16" s="52">
+        <v>0.09</v>
+      </c>
+      <c r="F16" s="52">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G16">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H16">
+        <v>0.08</v>
+      </c>
+      <c r="I16">
+        <v>0.16</v>
+      </c>
+      <c r="J16">
+        <v>0.1</v>
+      </c>
+      <c r="K16" s="52">
+        <v>0.08</v>
+      </c>
+      <c r="L16" s="52">
+        <v>0.01</v>
+      </c>
+      <c r="M16">
+        <v>0.01</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0.01</v>
+      </c>
+      <c r="Q16">
+        <v>0.04</v>
+      </c>
+      <c r="R16">
+        <v>0.04</v>
+      </c>
+      <c r="S16">
+        <v>0.04</v>
+      </c>
+      <c r="T16">
+        <v>0.02</v>
+      </c>
+      <c r="U16">
+        <v>0.02</v>
+      </c>
+      <c r="V16">
+        <v>0.03</v>
+      </c>
+      <c r="W16">
+        <v>0.02</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="52">
+        <v>0.03</v>
+      </c>
+      <c r="F17" s="52">
+        <v>0.05</v>
+      </c>
+      <c r="G17">
+        <v>0.09</v>
+      </c>
+      <c r="H17">
+        <v>0.11</v>
+      </c>
+      <c r="I17">
+        <v>0.12</v>
+      </c>
+      <c r="J17">
+        <v>0.1</v>
+      </c>
+      <c r="K17" s="52">
+        <v>0.09</v>
+      </c>
+      <c r="L17" s="52">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M17">
+        <v>0.05</v>
+      </c>
+      <c r="N17">
+        <v>0.01</v>
+      </c>
+      <c r="O17">
+        <v>0.01</v>
+      </c>
+      <c r="P17">
+        <v>0.01</v>
+      </c>
+      <c r="Q17">
+        <v>0.03</v>
+      </c>
+      <c r="R17">
+        <v>0.05</v>
+      </c>
+      <c r="S17">
+        <v>0.05</v>
+      </c>
+      <c r="T17">
+        <v>0.04</v>
+      </c>
+      <c r="U17">
+        <v>0.04</v>
+      </c>
+      <c r="V17">
+        <v>0.02</v>
+      </c>
+      <c r="W17">
+        <v>0.01</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="B18">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C18">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="D18">
+        <v>0.13</v>
+      </c>
+      <c r="E18" s="52">
+        <v>0.106</v>
+      </c>
+      <c r="F18" s="52">
+        <v>9.4E-2</v>
+      </c>
+      <c r="G18">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="H18">
+        <v>0.109</v>
+      </c>
+      <c r="I18">
+        <v>0.127</v>
+      </c>
+      <c r="J18">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="K18" s="52">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="L18" s="52">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N18">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="O18">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="P18">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="Q18">
+        <v>0.02</v>
+      </c>
+      <c r="R18">
+        <v>0.01</v>
+      </c>
+      <c r="S18">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="T18">
+        <v>2E-3</v>
+      </c>
+      <c r="U18">
+        <v>1E-3</v>
+      </c>
+      <c r="V18">
+        <v>1E-3</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0.01</v>
+      </c>
+      <c r="D19">
+        <v>0.03</v>
+      </c>
+      <c r="E19">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F19">
+        <v>0.12</v>
+      </c>
+      <c r="G19">
+        <v>0.13</v>
+      </c>
+      <c r="H19">
+        <v>0.16</v>
+      </c>
+      <c r="I19">
+        <v>0.16</v>
+      </c>
+      <c r="J19">
+        <v>0.12</v>
+      </c>
+      <c r="K19">
+        <v>0.06</v>
+      </c>
+      <c r="L19">
+        <v>0.02</v>
+      </c>
+      <c r="M19">
+        <v>0.01</v>
+      </c>
+      <c r="N19">
+        <v>0.01</v>
+      </c>
+      <c r="O19">
+        <v>0.02</v>
+      </c>
+      <c r="P19">
+        <v>0.01</v>
+      </c>
+      <c r="Q19">
+        <v>0.01</v>
+      </c>
+      <c r="R19">
+        <v>0.02</v>
+      </c>
+      <c r="S19">
+        <v>0.02</v>
+      </c>
+      <c r="T19">
+        <v>0.01</v>
+      </c>
+      <c r="U19">
+        <v>0.01</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>3.49E-2</v>
+      </c>
+      <c r="F20">
+        <v>2.3800000000000002E-2</v>
+      </c>
+      <c r="G20">
+        <v>2.3300000000000001E-2</v>
+      </c>
+      <c r="H20">
+        <v>1.44E-2</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="K20">
+        <v>1.9E-3</v>
+      </c>
+      <c r="L20">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="M20">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="N20">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="O20">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="P20">
+        <v>2.69E-2</v>
+      </c>
+      <c r="Q20">
+        <v>6.88E-2</v>
+      </c>
+      <c r="R20">
+        <v>0.15060000000000001</v>
+      </c>
+      <c r="S20">
+        <v>0.1507</v>
+      </c>
+      <c r="T20">
+        <v>0.1431</v>
+      </c>
+      <c r="U20">
+        <v>0.12280000000000001</v>
+      </c>
+      <c r="V20">
+        <v>7.85E-2</v>
+      </c>
+      <c r="W20">
+        <v>7.8299999999999995E-2</v>
+      </c>
+      <c r="X20">
+        <v>2.29E-2</v>
+      </c>
+      <c r="Y20">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="Z20">
+        <v>1E-3</v>
+      </c>
+      <c r="AA20">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="AB20">
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1E-3</v>
+      </c>
+      <c r="E21">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F21">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="G21">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="H21">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I21">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="J21">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="K21">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="L21">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M21">
+        <v>2.4E-2</v>
+      </c>
+      <c r="N21">
+        <v>1.2E-2</v>
+      </c>
+      <c r="O21">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="P21">
+        <v>1.6E-2</v>
+      </c>
+      <c r="Q21">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="R21">
+        <v>1.6E-2</v>
+      </c>
+      <c r="S21">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="T21">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="U21">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="V21">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="W21">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="X21">
+        <v>6.3E-2</v>
+      </c>
+      <c r="Y21">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="Z21">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AA21">
+        <v>1E-3</v>
+      </c>
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1204860-D74C-4820-9105-F5F83CDB7EC9}">
   <dimension ref="A3:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
@@ -6722,38 +9405,38 @@
       <c r="A24" s="28">
         <v>2006</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43">
+      <c r="B24" s="38"/>
+      <c r="C24" s="38">
         <v>8383.58</v>
       </c>
-      <c r="D24" s="43">
+      <c r="D24" s="38">
         <v>7485.28</v>
       </c>
-      <c r="E24" s="43">
+      <c r="E24" s="38">
         <v>2008.11</v>
       </c>
-      <c r="F24" s="43">
+      <c r="F24" s="38">
         <v>3409.69</v>
       </c>
-      <c r="G24" s="43">
+      <c r="G24" s="38">
         <v>2760.07</v>
       </c>
-      <c r="H24" s="43">
+      <c r="H24" s="38">
         <v>3285.78</v>
       </c>
-      <c r="I24" s="43">
+      <c r="I24" s="38">
         <v>722.51</v>
       </c>
-      <c r="J24" s="43">
+      <c r="J24" s="38">
         <v>367.07</v>
       </c>
-      <c r="K24" s="43">
+      <c r="K24" s="38">
         <v>2884.61</v>
       </c>
-      <c r="L24" s="43">
+      <c r="L24" s="38">
         <v>2822.19</v>
       </c>
-      <c r="M24" s="43">
+      <c r="M24" s="38">
         <v>1830.5</v>
       </c>
     </row>
@@ -6761,77 +9444,77 @@
       <c r="A25" s="28">
         <v>2007</v>
       </c>
-      <c r="B25" s="43">
+      <c r="B25" s="38">
         <v>5739.74</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C25" s="38">
         <v>5100.67</v>
       </c>
-      <c r="D25" s="43">
+      <c r="D25" s="38">
         <v>4180.8999999999996</v>
       </c>
-      <c r="E25" s="43">
+      <c r="E25" s="38">
         <v>4651.16</v>
       </c>
-      <c r="F25" s="43">
+      <c r="F25" s="38">
         <v>7430.22</v>
       </c>
-      <c r="G25" s="43">
+      <c r="G25" s="38">
         <v>4694.1499999999996</v>
       </c>
-      <c r="H25" s="43">
+      <c r="H25" s="38">
         <v>3027.25</v>
       </c>
-      <c r="I25" s="43">
+      <c r="I25" s="38">
         <v>3717.74</v>
       </c>
-      <c r="J25" s="43">
+      <c r="J25" s="38">
         <v>16.989999999999998</v>
       </c>
-      <c r="K25" s="43">
+      <c r="K25" s="38">
         <v>1821.76</v>
       </c>
-      <c r="L25" s="43">
+      <c r="L25" s="38">
         <v>4092.69</v>
       </c>
-      <c r="M25" s="43"/>
+      <c r="M25" s="38"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A26" s="28">
         <v>2008</v>
       </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43">
+      <c r="B26" s="38"/>
+      <c r="C26" s="38">
         <v>10122.34</v>
       </c>
-      <c r="D26" s="43">
+      <c r="D26" s="38">
         <v>6489.43</v>
       </c>
-      <c r="E26" s="43">
+      <c r="E26" s="38">
         <v>4329.05</v>
       </c>
-      <c r="F26" s="43">
+      <c r="F26" s="38">
         <v>4822.78</v>
       </c>
-      <c r="G26" s="43">
+      <c r="G26" s="38">
         <v>951.18</v>
       </c>
-      <c r="H26" s="43">
+      <c r="H26" s="38">
         <v>282.13</v>
       </c>
-      <c r="I26" s="43">
+      <c r="I26" s="38">
         <v>13.12</v>
       </c>
-      <c r="J26" s="43">
+      <c r="J26" s="38">
         <v>34.49</v>
       </c>
-      <c r="K26" s="43">
+      <c r="K26" s="38">
         <v>7046.08</v>
       </c>
-      <c r="L26" s="43">
+      <c r="L26" s="38">
         <v>5954.34</v>
       </c>
-      <c r="M26" s="43">
+      <c r="M26" s="38">
         <v>5034.7299999999996</v>
       </c>
     </row>
@@ -6839,36 +9522,36 @@
       <c r="A27" s="28">
         <v>2009</v>
       </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43">
+      <c r="B27" s="38"/>
+      <c r="C27" s="38">
         <v>4.66</v>
       </c>
-      <c r="D27" s="43">
+      <c r="D27" s="38">
         <v>9488.36</v>
       </c>
-      <c r="E27" s="43">
+      <c r="E27" s="38">
         <v>13247.21</v>
       </c>
-      <c r="F27" s="43">
+      <c r="F27" s="38">
         <v>9750.19</v>
       </c>
-      <c r="G27" s="43">
+      <c r="G27" s="38">
         <v>6552.63</v>
       </c>
-      <c r="H27" s="43">
+      <c r="H27" s="38">
         <v>4406.54</v>
       </c>
-      <c r="I27" s="43">
+      <c r="I27" s="38">
         <v>1514.02</v>
       </c>
-      <c r="J27" s="43">
+      <c r="J27" s="38">
         <v>88.03</v>
       </c>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43">
+      <c r="K27" s="38"/>
+      <c r="L27" s="38">
         <v>1814.46</v>
       </c>
-      <c r="M27" s="43">
+      <c r="M27" s="38">
         <v>2356.04</v>
       </c>
     </row>
@@ -6876,38 +9559,38 @@
       <c r="A28" s="28">
         <v>2010</v>
       </c>
-      <c r="B28" s="43">
+      <c r="B28" s="38">
         <v>163.85</v>
       </c>
-      <c r="C28" s="43">
+      <c r="C28" s="38">
         <v>1444.99</v>
       </c>
-      <c r="D28" s="43">
+      <c r="D28" s="38">
         <v>6826</v>
       </c>
-      <c r="E28" s="43">
+      <c r="E28" s="38">
         <v>3397.09</v>
       </c>
-      <c r="F28" s="43">
+      <c r="F28" s="38">
         <v>4685.6899999999996</v>
       </c>
-      <c r="G28" s="43">
+      <c r="G28" s="38">
         <v>1563.73</v>
       </c>
-      <c r="H28" s="43">
+      <c r="H28" s="38">
         <v>179.9</v>
       </c>
-      <c r="I28" s="43">
+      <c r="I28" s="38">
         <v>56.37</v>
       </c>
-      <c r="J28" s="43">
+      <c r="J28" s="38">
         <v>143.06</v>
       </c>
-      <c r="K28" s="43"/>
-      <c r="L28" s="43">
+      <c r="K28" s="38"/>
+      <c r="L28" s="38">
         <v>757.77</v>
       </c>
-      <c r="M28" s="43">
+      <c r="M28" s="38">
         <v>1005.69</v>
       </c>
     </row>
@@ -6915,40 +9598,40 @@
       <c r="A29" s="28">
         <v>2011</v>
       </c>
-      <c r="B29" s="43">
+      <c r="B29" s="38">
         <v>623.38</v>
       </c>
-      <c r="C29" s="43">
+      <c r="C29" s="38">
         <v>279.48</v>
       </c>
-      <c r="D29" s="43">
+      <c r="D29" s="38">
         <v>2887.18</v>
       </c>
-      <c r="E29" s="43">
+      <c r="E29" s="38">
         <v>2785.13</v>
       </c>
-      <c r="F29" s="43">
+      <c r="F29" s="38">
         <v>3743.68</v>
       </c>
-      <c r="G29" s="43">
+      <c r="G29" s="38">
         <v>700.44</v>
       </c>
-      <c r="H29" s="43">
+      <c r="H29" s="38">
         <v>52.63</v>
       </c>
-      <c r="I29" s="43">
+      <c r="I29" s="38">
         <v>111.37</v>
       </c>
-      <c r="J29" s="43">
+      <c r="J29" s="38">
         <v>20.69</v>
       </c>
-      <c r="K29" s="43">
+      <c r="K29" s="38">
         <v>13.5</v>
       </c>
-      <c r="L29" s="43">
+      <c r="L29" s="38">
         <v>2026.73</v>
       </c>
-      <c r="M29" s="43">
+      <c r="M29" s="38">
         <v>3549.19</v>
       </c>
     </row>
@@ -6956,34 +9639,34 @@
       <c r="A30" s="28">
         <v>2012</v>
       </c>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43">
+      <c r="B30" s="38"/>
+      <c r="C30" s="38">
         <v>3854.56</v>
       </c>
-      <c r="D30" s="43">
+      <c r="D30" s="38">
         <v>3189.61</v>
       </c>
-      <c r="E30" s="43">
+      <c r="E30" s="38">
         <v>2151.48</v>
       </c>
-      <c r="F30" s="43">
+      <c r="F30" s="38">
         <v>1192.5999999999999</v>
       </c>
-      <c r="G30" s="43">
+      <c r="G30" s="38">
         <v>2160.14</v>
       </c>
-      <c r="H30" s="43">
+      <c r="H30" s="38">
         <v>6521.21</v>
       </c>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="43">
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38">
         <v>2.7</v>
       </c>
-      <c r="L30" s="43">
+      <c r="L30" s="38">
         <v>4.37</v>
       </c>
-      <c r="M30" s="43">
+      <c r="M30" s="38">
         <v>642.46</v>
       </c>
     </row>
@@ -6991,40 +9674,40 @@
       <c r="A31" s="28">
         <v>2013</v>
       </c>
-      <c r="B31" s="43">
+      <c r="B31" s="38">
         <v>825.51</v>
       </c>
-      <c r="C31" s="43">
+      <c r="C31" s="38">
         <v>6453.63</v>
       </c>
-      <c r="D31" s="43">
+      <c r="D31" s="38">
         <v>5252.1</v>
       </c>
-      <c r="E31" s="43">
+      <c r="E31" s="38">
         <v>1975.77</v>
       </c>
-      <c r="F31" s="43">
+      <c r="F31" s="38">
         <v>300.24</v>
       </c>
-      <c r="G31" s="43">
+      <c r="G31" s="38">
         <v>637.26</v>
       </c>
-      <c r="H31" s="43">
+      <c r="H31" s="38">
         <v>618.19000000000005</v>
       </c>
-      <c r="I31" s="43">
+      <c r="I31" s="38">
         <v>737.25</v>
       </c>
-      <c r="J31" s="43">
+      <c r="J31" s="38">
         <v>240.11</v>
       </c>
-      <c r="K31" s="43">
+      <c r="K31" s="38">
         <v>220.4</v>
       </c>
-      <c r="L31" s="43">
+      <c r="L31" s="38">
         <v>1776.02</v>
       </c>
-      <c r="M31" s="43">
+      <c r="M31" s="38">
         <v>2715.49</v>
       </c>
     </row>
@@ -7032,40 +9715,40 @@
       <c r="A32" s="28">
         <v>2014</v>
       </c>
-      <c r="B32" s="43">
+      <c r="B32" s="38">
         <v>1087.25</v>
       </c>
-      <c r="C32" s="43">
+      <c r="C32" s="38">
         <v>3299.37</v>
       </c>
-      <c r="D32" s="43">
+      <c r="D32" s="38">
         <v>4283.62</v>
       </c>
-      <c r="E32" s="43">
+      <c r="E32" s="38">
         <v>756.45</v>
       </c>
-      <c r="F32" s="43">
+      <c r="F32" s="38">
         <v>1821.83</v>
       </c>
-      <c r="G32" s="43">
+      <c r="G32" s="38">
         <v>1877.35</v>
       </c>
-      <c r="H32" s="43">
+      <c r="H32" s="38">
         <v>2677.82</v>
       </c>
-      <c r="I32" s="43">
+      <c r="I32" s="38">
         <v>354.41</v>
       </c>
-      <c r="J32" s="43">
+      <c r="J32" s="38">
         <v>43.05</v>
       </c>
-      <c r="K32" s="43">
+      <c r="K32" s="38">
         <v>174.95</v>
       </c>
-      <c r="L32" s="43">
+      <c r="L32" s="38">
         <v>2721.73</v>
       </c>
-      <c r="M32" s="43">
+      <c r="M32" s="38">
         <v>3680.93</v>
       </c>
     </row>
@@ -7073,40 +9756,40 @@
       <c r="A33" s="28">
         <v>2015</v>
       </c>
-      <c r="B33" s="43">
+      <c r="B33" s="38">
         <v>9087.5</v>
       </c>
-      <c r="C33" s="43">
+      <c r="C33" s="38">
         <v>5533.01</v>
       </c>
-      <c r="D33" s="43">
+      <c r="D33" s="38">
         <v>4602.96</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="38">
         <v>8.16</v>
       </c>
-      <c r="F33" s="43">
+      <c r="F33" s="38">
         <v>116.41</v>
       </c>
-      <c r="G33" s="43">
+      <c r="G33" s="38">
         <v>665.38</v>
       </c>
-      <c r="H33" s="43">
+      <c r="H33" s="38">
         <v>365.26</v>
       </c>
-      <c r="I33" s="43">
+      <c r="I33" s="38">
         <v>65.150000000000006</v>
       </c>
-      <c r="J33" s="43">
+      <c r="J33" s="38">
         <v>41.6</v>
       </c>
-      <c r="K33" s="43">
+      <c r="K33" s="38">
         <v>58.71</v>
       </c>
-      <c r="L33" s="43">
+      <c r="L33" s="38">
         <v>66.12</v>
       </c>
-      <c r="M33" s="43">
+      <c r="M33" s="38">
         <v>3100.47</v>
       </c>
     </row>
@@ -7114,40 +9797,40 @@
       <c r="A34" s="28">
         <v>2016</v>
       </c>
-      <c r="B34" s="43">
+      <c r="B34" s="38">
         <v>2523.4299999999998</v>
       </c>
-      <c r="C34" s="43">
+      <c r="C34" s="38">
         <v>6361.81</v>
       </c>
-      <c r="D34" s="43">
+      <c r="D34" s="38">
         <v>738.8</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E34" s="38">
         <v>1714.5</v>
       </c>
-      <c r="F34" s="43">
+      <c r="F34" s="38">
         <v>569.44000000000005</v>
       </c>
-      <c r="G34" s="43">
+      <c r="G34" s="38">
         <v>1697.93</v>
       </c>
-      <c r="H34" s="43">
+      <c r="H34" s="38">
         <v>870.99</v>
       </c>
-      <c r="I34" s="43">
+      <c r="I34" s="38">
         <v>133.82</v>
       </c>
-      <c r="J34" s="43">
+      <c r="J34" s="38">
         <v>37.4</v>
       </c>
-      <c r="K34" s="43">
+      <c r="K34" s="38">
         <v>62.09</v>
       </c>
-      <c r="L34" s="43">
+      <c r="L34" s="38">
         <v>85.53</v>
       </c>
-      <c r="M34" s="43">
+      <c r="M34" s="38">
         <v>3663.88</v>
       </c>
     </row>
@@ -7155,40 +9838,40 @@
       <c r="A35" s="28">
         <v>2017</v>
       </c>
-      <c r="B35" s="43">
+      <c r="B35" s="38">
         <v>531.4</v>
       </c>
-      <c r="C35" s="43">
+      <c r="C35" s="38">
         <v>1279.81</v>
       </c>
-      <c r="D35" s="43">
+      <c r="D35" s="38">
         <v>2858.19</v>
       </c>
-      <c r="E35" s="43">
+      <c r="E35" s="38">
         <v>61.4</v>
       </c>
-      <c r="F35" s="43">
+      <c r="F35" s="38">
         <v>2424.86</v>
       </c>
-      <c r="G35" s="43">
+      <c r="G35" s="38">
         <v>1858.42</v>
       </c>
-      <c r="H35" s="43">
+      <c r="H35" s="38">
         <v>946.56</v>
       </c>
-      <c r="I35" s="43">
+      <c r="I35" s="38">
         <v>608.99</v>
       </c>
-      <c r="J35" s="43">
+      <c r="J35" s="38">
         <v>91.44</v>
       </c>
-      <c r="K35" s="43">
+      <c r="K35" s="38">
         <v>103.23</v>
       </c>
-      <c r="L35" s="43">
+      <c r="L35" s="38">
         <v>913.13</v>
       </c>
-      <c r="M35" s="43">
+      <c r="M35" s="38">
         <v>2456.11</v>
       </c>
     </row>
@@ -7196,40 +9879,40 @@
       <c r="A36" s="28">
         <v>2018</v>
       </c>
-      <c r="B36" s="43">
+      <c r="B36" s="38">
         <v>125.6</v>
       </c>
-      <c r="C36" s="43">
+      <c r="C36" s="38">
         <v>22.15</v>
       </c>
-      <c r="D36" s="43">
+      <c r="D36" s="38">
         <v>48.46</v>
       </c>
-      <c r="E36" s="43">
+      <c r="E36" s="38">
         <v>74.03</v>
       </c>
-      <c r="F36" s="43">
+      <c r="F36" s="38">
         <v>494.86</v>
       </c>
-      <c r="G36" s="43">
+      <c r="G36" s="38">
         <v>870.48</v>
       </c>
-      <c r="H36" s="43">
+      <c r="H36" s="38">
         <v>954.53</v>
       </c>
-      <c r="I36" s="43">
+      <c r="I36" s="38">
         <v>650.89</v>
       </c>
-      <c r="J36" s="43">
+      <c r="J36" s="38">
         <v>687.59</v>
       </c>
-      <c r="K36" s="43">
+      <c r="K36" s="38">
         <v>61.46</v>
       </c>
-      <c r="L36" s="43">
+      <c r="L36" s="38">
         <v>1121.5899999999999</v>
       </c>
-      <c r="M36" s="43">
+      <c r="M36" s="38">
         <v>3243.74</v>
       </c>
     </row>
@@ -7237,40 +9920,40 @@
       <c r="A37" s="28">
         <v>2019</v>
       </c>
-      <c r="B37" s="43">
+      <c r="B37" s="38">
         <v>2456.46</v>
       </c>
-      <c r="C37" s="43">
+      <c r="C37" s="38">
         <v>1523.62</v>
       </c>
-      <c r="D37" s="43">
+      <c r="D37" s="38">
         <v>1218.04</v>
       </c>
-      <c r="E37" s="43">
+      <c r="E37" s="38">
         <v>145.13</v>
       </c>
-      <c r="F37" s="43">
+      <c r="F37" s="38">
         <v>483.09</v>
       </c>
-      <c r="G37" s="43">
+      <c r="G37" s="38">
         <v>769.66</v>
       </c>
-      <c r="H37" s="43">
+      <c r="H37" s="38">
         <v>1430.74</v>
       </c>
-      <c r="I37" s="43">
+      <c r="I37" s="38">
         <v>520.37</v>
       </c>
-      <c r="J37" s="43">
+      <c r="J37" s="38">
         <v>20.29</v>
       </c>
-      <c r="K37" s="43">
+      <c r="K37" s="38">
         <v>182.38</v>
       </c>
-      <c r="L37" s="43">
+      <c r="L37" s="38">
         <v>1055.93</v>
       </c>
-      <c r="M37" s="43">
+      <c r="M37" s="38">
         <v>1463.63</v>
       </c>
     </row>
@@ -7278,40 +9961,40 @@
       <c r="A38" s="28">
         <v>2020</v>
       </c>
-      <c r="B38" s="43">
+      <c r="B38" s="38">
         <v>1898.52</v>
       </c>
-      <c r="C38" s="43">
+      <c r="C38" s="38">
         <v>2100.77</v>
       </c>
-      <c r="D38" s="43">
+      <c r="D38" s="38">
         <v>1026.93</v>
       </c>
-      <c r="E38" s="43">
+      <c r="E38" s="38">
         <v>15.2</v>
       </c>
-      <c r="F38" s="43">
+      <c r="F38" s="38">
         <v>326.11</v>
       </c>
-      <c r="G38" s="43">
+      <c r="G38" s="38">
         <v>109.77</v>
       </c>
-      <c r="H38" s="43">
+      <c r="H38" s="38">
         <v>464.81</v>
       </c>
-      <c r="I38" s="43">
+      <c r="I38" s="38">
         <v>337.21</v>
       </c>
-      <c r="J38" s="43">
+      <c r="J38" s="38">
         <v>87.46</v>
       </c>
-      <c r="K38" s="43">
+      <c r="K38" s="38">
         <v>79.650000000000006</v>
       </c>
-      <c r="L38" s="43">
+      <c r="L38" s="38">
         <v>3063.82</v>
       </c>
-      <c r="M38" s="43">
+      <c r="M38" s="38">
         <v>4683.49</v>
       </c>
     </row>
@@ -7319,28 +10002,28 @@
       <c r="A39" s="28">
         <v>2021</v>
       </c>
-      <c r="B39" s="43">
+      <c r="B39" s="38">
         <v>1161.81</v>
       </c>
-      <c r="C39" s="43">
+      <c r="C39" s="38">
         <v>3102.61</v>
       </c>
-      <c r="D39" s="43">
+      <c r="D39" s="38">
         <v>1844.82</v>
       </c>
-      <c r="E39" s="43">
+      <c r="E39" s="38">
         <v>92.53</v>
       </c>
-      <c r="F39" s="43">
+      <c r="F39" s="38">
         <v>29.44</v>
       </c>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="43"/>
-      <c r="L39" s="43"/>
-      <c r="M39" s="43"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="38"/>
+      <c r="K39" s="38"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>